<commit_message>
Fix strings based on localization review
</commit_message>
<xml_diff>
--- a/Workbooks/JA/キュー.xlsx
+++ b/Workbooks/JA/キュー.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD96EC7-DDBB-4697-915F-0A96A9D83C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1705B9FC-5A23-4267-8D94-52A68D170E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="取得" sheetId="4" r:id="rId1"/>
     <sheet name="作成" sheetId="1" r:id="rId2"/>
     <sheet name="削除" sheetId="2" r:id="rId3"/>
-    <sheet name="キューアイテムをダウンロード" sheetId="6" r:id="rId4"/>
-    <sheet name="キューアイテムをアップロード" sheetId="7" r:id="rId5"/>
+    <sheet name="キュー アイテムをダウンロード" sheetId="6" r:id="rId4"/>
+    <sheet name="キュー アイテムをアップロード" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -332,12 +332,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -889,24 +883,9 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1101,6 +1080,27 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1115,75 +1115,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H201" headerRowDxfId="32" dataDxfId="30" totalsRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H201" headerRowDxfId="40" dataDxfId="39" totalsRowDxfId="38">
   <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{F48D04D3-B22E-457E-8F3F-6D0CF14127A6}" name="フォルダーID" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{012AE434-BA00-4CDD-8DBE-8524E276CBF0}" name="フォルダー名" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{81F10BAB-541D-4EEA-8F4A-504125FC59D3}" name="キューID" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="キュー名" totalsRowLabel="Total" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="説明" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="一意の参照" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{EA8DF354-2F10-4E45-801A-56D5F80552D8}" name="自動リトライ" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="最大リトライ回数" totalsRowFunction="count" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{F48D04D3-B22E-457E-8F3F-6D0CF14127A6}" name="フォルダーID" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{012AE434-BA00-4CDD-8DBE-8524E276CBF0}" name="フォルダー名" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{81F10BAB-541D-4EEA-8F4A-504125FC59D3}" name="キューID" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="キュー名" totalsRowLabel="Total" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="説明" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="一意の参照" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{EA8DF354-2F10-4E45-801A-56D5F80552D8}" name="自動リトライ" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="最大リトライ回数" totalsRowFunction="count" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H201" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H201" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{3C3B66B3-BB87-4C07-80BD-579ABFE71137}" name="フォルダー名" dataDxfId="29"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="キュー名" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="説明" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="一意の参照" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{07A3D78A-00F5-4019-BC61-B83E2CEDEEA5}" name="自動リトライ" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{5CA1824C-85AD-40DB-A0CE-9853C443448E}" name="最大リトライ回数" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="結果" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{3C3B66B3-BB87-4C07-80BD-579ABFE71137}" name="フォルダー名" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="キュー名" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="説明" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="一意の参照" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{07A3D78A-00F5-4019-BC61-B83E2CEDEEA5}" name="自動リトライ" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{5CA1824C-85AD-40DB-A0CE-9853C443448E}" name="最大リトライ回数" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="結果" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{2E1B6A8E-85FA-465E-B215-15A8D8C44B57}" name="フォルダーID" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{5CFD4745-18D2-4B9F-9127-E66CA25B38B2}" name="フォルダー名" dataDxfId="18"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="キューID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="キュー名" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="結果" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{2E1B6A8E-85FA-465E-B215-15A8D8C44B57}" name="フォルダーID" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{5CFD4745-18D2-4B9F-9127-E66CA25B38B2}" name="フォルダー名" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="キューID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="キュー名" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="結果" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BDD2F9DC-3028-471A-A247-2ED5A9AC5566}" name="Table135" displayName="Table135" ref="A1:D201" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BDD2F9DC-3028-471A-A247-2ED5A9AC5566}" name="Table135" displayName="Table135" ref="A1:D201" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{3A524577-2886-46D9-BDC3-73F7E697D198}" name="フォルダー名" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{FAB26460-45C9-47D7-93FB-35118D5F4DF0}" name="キュー名" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{C455FEB9-1F4C-4FD2-9BC3-F5CA89B885F6}" name="保存フォルダーパス" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{EDEDFBDB-A6F3-441B-AA68-79FEE4009BFD}" name="結果" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{3A524577-2886-46D9-BDC3-73F7E697D198}" name="フォルダー名" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{FAB26460-45C9-47D7-93FB-35118D5F4DF0}" name="キュー名" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{C455FEB9-1F4C-4FD2-9BC3-F5CA89B885F6}" name="保存フォルダーパス" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{EDEDFBDB-A6F3-441B-AA68-79FEE4009BFD}" name="結果" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C4F260B6-262D-46C1-B4D1-BCFC6884B63D}" name="Table1356" displayName="Table1356" ref="A1:E201" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C4F260B6-262D-46C1-B4D1-BCFC6884B63D}" name="Table1356" displayName="Table1356" ref="A1:E201" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{F1E05E03-DBDF-4491-9EE8-8A6B21F57814}" name="フォルダー名" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{E328AFBB-DF63-41AD-B11E-E7642D9A3121}" name="キュー名" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{56CE4921-90D7-421E-9313-6592D86EA9FB}" name="キューアイテム一覧のファイルパス" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{32C7ACF1-5123-4602-B742-646D45AF8932}" name="コミットの種類" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{835CC962-3DD4-4C84-9423-395F4642CE78}" name="結果" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F1E05E03-DBDF-4491-9EE8-8A6B21F57814}" name="フォルダー名" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E328AFBB-DF63-41AD-B11E-E7642D9A3121}" name="キュー名" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{56CE4921-90D7-421E-9313-6592D86EA9FB}" name="キューアイテム一覧のファイルパス" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{32C7ACF1-5123-4602-B742-646D45AF8932}" name="コミットの種類" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{835CC962-3DD4-4C84-9423-395F4642CE78}" name="結果" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Refactor migration of Assets per Robot from Classic to Modern Folders
</commit_message>
<xml_diff>
--- a/Workbooks/JA/キュー.xlsx
+++ b/Workbooks/JA/キュー.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C073B30-28F8-47B5-951C-38F2B0994721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966A367A-EE8B-4292-8D8C-650687A7BFC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>
@@ -1460,13 +1460,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" style="15" customWidth="1"/>
     <col min="4" max="4" width="25.6328125" style="10" customWidth="1"/>
     <col min="5" max="5" width="45.6328125" style="10" customWidth="1"/>
     <col min="6" max="6" width="25.6328125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.6328125" style="16" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="10"/>
   </cols>
@@ -3533,7 +3533,7 @@
     <col min="1" max="2" width="25.6328125" style="5" customWidth="1"/>
     <col min="3" max="3" width="45.6328125" style="21" customWidth="1"/>
     <col min="4" max="4" width="25.6328125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.6328125" style="10" customWidth="1"/>
     <col min="7" max="7" width="15.6328125" style="10" customWidth="1"/>
     <col min="8" max="8" width="45.6328125" style="10" customWidth="1"/>
@@ -5597,7 +5597,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" style="10" customWidth="1"/>
     <col min="4" max="4" width="25.6328125" style="10" customWidth="1"/>

</xml_diff>

<commit_message>
JP-1473: Support description for Assets
</commit_message>
<xml_diff>
--- a/Workbooks/JA/キュー.xlsx
+++ b/Workbooks/JA/キュー.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryota.okuji\Documents\UiPath\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B334CC-00F5-4D9F-8537-96F77374592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8698491C-92A2-4284-9F71-69038A4677FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61575" yWindow="1260" windowWidth="23640" windowHeight="12630" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="取得" sheetId="4" r:id="rId1"/>

</xml_diff>